<commit_message>
add some new plot
</commit_message>
<xml_diff>
--- a/Data/Plot/baseline_timing.xlsx
+++ b/Data/Plot/baseline_timing.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eth\asl\team42\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eth\asl\team42\Data\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCD183F-1455-43EE-A7C9-3C4EACAB3D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF64D33E-C7EB-4D58-9133-CBBA31223CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1F9DB3D-A5ED-4CF3-8993-B9AA5F6B7807}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B1F9DB3D-A5ED-4CF3-8993-B9AA5F6B7807}"/>
   </bookViews>
   <sheets>
-    <sheet name="baseline" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="baseline" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>cycles</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +77,26 @@
   </si>
   <si>
     <t>radius=0.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocking_v1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocking_v2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 * 5 * 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vectorization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -202,7 +223,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -231,6 +252,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -272,6 +296,894 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>图表标题</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.2886482939632541E-2"/>
+          <c:y val="0.30650886626976503"/>
+          <c:w val="0.87755796150481191"/>
+          <c:h val="0.50916848046433216"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$15:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.42965625E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16179062499999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49349375000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1009387500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0795224999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4677349999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4661150000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0607199999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.434855000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.565754999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-900E-420C-A463-E23C337E87A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>blocking_v1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$15:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$15:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.1115898437500001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27267093749999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78487375000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7038599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1236799999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1012199999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1065000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.798970000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.688205</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.701944999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-900E-420C-A463-E23C337E87A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>blocking_v2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$15:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.1624296874999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2380721875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67800687500000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5105012499999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8056274999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6335449999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3252350000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.770210000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.183305000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.707450000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-106B-41A9-B22E-BE6F23A68984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vectorization</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$15:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$15:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0510683593749999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11781343750000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34157468749999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72119437500000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0612712500000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8493174999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0345650000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6309199999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.052365</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4201549999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-106B-41A9-B22E-BE6F23A68984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="526523984"/>
+        <c:axId val="526520376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="526523984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US"/>
+                  <a:t>标题</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="526520376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="526520376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="526523984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72448676919770993"/>
+          <c:y val="0.40989106544608761"/>
+          <c:w val="0.24363714269322892"/>
+          <c:h val="0.32774470264387684"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -1060,6 +1972,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1576,7 +2528,625 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>906780</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087273F3-5F1D-82A8-F8D7-3E20C8C471DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.18956</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.2</cdr:x>
+      <cdr:y>0.52289</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="文本框 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EECBD7F5-6EB2-6441-0030-BFEE2D2FBA16}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="519998"/>
+          <a:ext cx="914400" cy="914391"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>[ms]</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1617,7 +3187,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -1974,11 +3544,459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1E943F-ED1A-427E-B4E0-8AD265FB7C11}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9">
+        <v>68030.375</v>
+      </c>
+      <c r="C3" s="9">
+        <v>87124.515625</v>
+      </c>
+      <c r="D3" s="9">
+        <v>88548.03125</v>
+      </c>
+      <c r="E3" s="9">
+        <v>57429.9140625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9">
+        <v>453013.75</v>
+      </c>
+      <c r="C4" s="9">
+        <v>763478.625</v>
+      </c>
+      <c r="D4" s="9">
+        <v>666602.125</v>
+      </c>
+      <c r="E4" s="9">
+        <v>329877.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1381782.5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2197646.5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1898419.25</v>
+      </c>
+      <c r="E5" s="9">
+        <v>956409.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>40</v>
+      </c>
+      <c r="B6" s="9">
+        <v>3082628.5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4770808</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4229403.5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2019344.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>50</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5822663</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8746304</v>
+      </c>
+      <c r="D7" s="9">
+        <v>7855757</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2971559.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>60</v>
+      </c>
+      <c r="B8" s="9">
+        <v>9709658</v>
+      </c>
+      <c r="C8" s="9">
+        <v>14283416</v>
+      </c>
+      <c r="D8" s="9">
+        <v>12973926</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5178089</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>70</v>
+      </c>
+      <c r="B9" s="9">
+        <v>15305122</v>
+      </c>
+      <c r="C9" s="9">
+        <v>22698200</v>
+      </c>
+      <c r="D9" s="9">
+        <v>20510658</v>
+      </c>
+      <c r="E9" s="9">
+        <v>8496782</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>80</v>
+      </c>
+      <c r="B10" s="9">
+        <v>22570016</v>
+      </c>
+      <c r="C10" s="9">
+        <v>33037116</v>
+      </c>
+      <c r="D10" s="9">
+        <v>30156588</v>
+      </c>
+      <c r="E10" s="9">
+        <v>12966576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>90</v>
+      </c>
+      <c r="B11" s="9">
+        <v>32017594</v>
+      </c>
+      <c r="C11" s="9">
+        <v>46726974</v>
+      </c>
+      <c r="D11" s="9">
+        <v>42513254</v>
+      </c>
+      <c r="E11" s="9">
+        <v>16946622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>100</v>
+      </c>
+      <c r="B12" s="9">
+        <v>43584114</v>
+      </c>
+      <c r="C12" s="9">
+        <v>63565446</v>
+      </c>
+      <c r="D12" s="9">
+        <v>57980860</v>
+      </c>
+      <c r="E12" s="9">
+        <v>23576434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>10</v>
+      </c>
+      <c r="B15" s="9">
+        <f>B3/2800000</f>
+        <v>2.42965625E-2</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" ref="C15:E15" si="0">C3/2800000</f>
+        <v>3.1115898437500001E-2</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1624296874999999E-2</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0510683593749999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>20</v>
+      </c>
+      <c r="B16" s="9">
+        <f t="shared" ref="B16:E24" si="1">B4/2800000</f>
+        <v>0.16179062499999999</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.27267093749999999</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2380721875</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.11781343750000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>30</v>
+      </c>
+      <c r="B17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.49349375000000001</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.78487375000000004</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.67800687500000001</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.34157468749999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9">
+        <f t="shared" si="1"/>
+        <v>1.1009387500000001</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="1"/>
+        <v>1.7038599999999999</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="1"/>
+        <v>1.5105012499999999</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="1"/>
+        <v>0.72119437500000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>50</v>
+      </c>
+      <c r="B19" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0795224999999999</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="1"/>
+        <v>3.1236799999999998</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="1"/>
+        <v>2.8056274999999999</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0612712500000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>60</v>
+      </c>
+      <c r="B20" s="9">
+        <f t="shared" si="1"/>
+        <v>3.4677349999999998</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="1"/>
+        <v>5.1012199999999996</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="1"/>
+        <v>4.6335449999999998</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" si="1"/>
+        <v>1.8493174999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>70</v>
+      </c>
+      <c r="B21" s="9">
+        <f t="shared" si="1"/>
+        <v>5.4661150000000003</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="1"/>
+        <v>8.1065000000000005</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>7.3252350000000002</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" si="1"/>
+        <v>3.0345650000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>80</v>
+      </c>
+      <c r="B22" s="9">
+        <f t="shared" si="1"/>
+        <v>8.0607199999999999</v>
+      </c>
+      <c r="C22" s="9">
+        <f t="shared" si="1"/>
+        <v>11.798970000000001</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>10.770210000000001</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="1"/>
+        <v>4.6309199999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>90</v>
+      </c>
+      <c r="B23" s="9">
+        <f t="shared" si="1"/>
+        <v>11.434855000000001</v>
+      </c>
+      <c r="C23" s="9">
+        <f t="shared" si="1"/>
+        <v>16.688205</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>15.183305000000001</v>
+      </c>
+      <c r="E23" s="9">
+        <f t="shared" si="1"/>
+        <v>6.052365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>100</v>
+      </c>
+      <c r="B24" s="9">
+        <f t="shared" si="1"/>
+        <v>15.565754999999999</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="1"/>
+        <v>22.701944999999998</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="1"/>
+        <v>20.707450000000001</v>
+      </c>
+      <c r="E24" s="9">
+        <f t="shared" si="1"/>
+        <v>8.4201549999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E252F772-8BFF-4763-82E2-BAB23D65FFF3}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1998,45 +4016,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="13"/>
-      <c r="E2" s="10" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="14"/>
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="13"/>
-      <c r="E3" s="10" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="E3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2434,12 +4452,12 @@
         <f>B17/2800000000</f>
         <v>2.589197265625E-5</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -2452,12 +4470,12 @@
         <f t="shared" ref="C18:C26" si="2">B18/2800000000</f>
         <v>1.5819203124999999E-4</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -2470,12 +4488,12 @@
         <f t="shared" si="2"/>
         <v>4.9388250000000002E-4</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">

</xml_diff>